<commit_message>
fix: ajustes na estrutura
</commit_message>
<xml_diff>
--- a/data/inventario_maquinas.xlsx
+++ b/data/inventario_maquinas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -632,7 +632,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Nenhum</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
@@ -667,11 +667,14 @@
           <t>gustavo.marques</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>Registro</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>Dell Inc.</t>
@@ -735,7 +738,12 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Nenhum</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Não será trocada</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -758,114 +766,7 @@
           <t>GRUPOANGELUS</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ANGDTI-N10005</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>gustavo.marques</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Registro</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Dell Inc.</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>9HZ14G3</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Notebook</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Vostro 3400</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Microsoft Windows 10 Pro</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>11th Gen Intel(R) Core(TM) i5-1135G7 @ 2.40GHz</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>DDR4</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P4" t="n">
-        <v>15.73</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>237.82</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>SSD</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Nenhum</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>GRUPOANGELUS</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>